<commit_message>
Updated Experiment 02 Results.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Experimentos/02/Results.xlsx
+++ b/Documents/Experimentos/02/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Volunteers" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="56">
   <si>
     <t>Q3</t>
   </si>
@@ -52,15 +52,9 @@
     <t>b</t>
   </si>
   <si>
-    <t>Tiveram menos tempo para responder</t>
-  </si>
-  <si>
     <t>Branco</t>
   </si>
   <si>
-    <t>TEMPO</t>
-  </si>
-  <si>
     <t>Vencedor</t>
   </si>
   <si>
@@ -131,6 +125,66 @@
   </si>
   <si>
     <t>=</t>
+  </si>
+  <si>
+    <t>Without</t>
+  </si>
+  <si>
+    <t>With</t>
+  </si>
+  <si>
+    <t>TEMPO(Menor)</t>
+  </si>
+  <si>
+    <t>PS: Tiveram menos tempo para responder</t>
+  </si>
+  <si>
+    <t>Diogo</t>
+  </si>
+  <si>
+    <t>Beatriz</t>
+  </si>
+  <si>
+    <t>José</t>
+  </si>
+  <si>
+    <t>Ralf</t>
+  </si>
+  <si>
+    <t>Rafael</t>
+  </si>
+  <si>
+    <t>Fernando</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Vinicius</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Matheus</t>
+  </si>
+  <si>
+    <t>Braian</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Renan</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Guilherme</t>
+  </si>
+  <si>
+    <t>Anibal</t>
   </si>
 </sst>
 </file>
@@ -153,7 +207,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="5"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -204,7 +258,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -236,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -268,22 +322,37 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -580,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -593,211 +662,306 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -807,10 +971,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -818,7 +982,7 @@
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -844,11 +1008,11 @@
         <v>0</v>
       </c>
       <c r="I1" s="5">
-        <f>AVERAGE(B1:H1)</f>
+        <f t="shared" ref="I1:I7" si="0">AVERAGE(B1:H1)</f>
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:12">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -874,11 +1038,11 @@
         <v>0</v>
       </c>
       <c r="I2" s="5">
-        <f>AVERAGE(B2:H2)</f>
+        <f t="shared" si="0"/>
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:12">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -904,11 +1068,11 @@
         <v>0</v>
       </c>
       <c r="I3" s="5">
-        <f>AVERAGE(B3:H3)</f>
+        <f t="shared" si="0"/>
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -934,11 +1098,11 @@
         <v>0</v>
       </c>
       <c r="I4" s="8">
-        <f>AVERAGE(B4:H4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -964,11 +1128,11 @@
         <v>0</v>
       </c>
       <c r="I5" s="5">
-        <f>AVERAGE(B5:H5)</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -994,11 +1158,11 @@
         <v>0</v>
       </c>
       <c r="I6" s="5">
-        <f>AVERAGE(B6:H6)</f>
+        <f t="shared" si="0"/>
         <v>3.5714285714285712E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1024,11 +1188,11 @@
         <v>1</v>
       </c>
       <c r="I7" s="5">
-        <f>AVERAGE(B7:H7)</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1036,7 +1200,7 @@
         <v>1030</v>
       </c>
       <c r="C8" s="4">
-        <v>1010</v>
+        <v>1025</v>
       </c>
       <c r="D8" s="4">
         <v>1025</v>
@@ -1051,11 +1215,11 @@
         <v>1025</v>
       </c>
       <c r="H8" s="4">
-        <v>1010</v>
+        <v>1025</v>
       </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1063,7 +1227,7 @@
         <v>1060</v>
       </c>
       <c r="C9" s="4">
-        <v>1030</v>
+        <v>1045</v>
       </c>
       <c r="D9" s="4">
         <v>1057</v>
@@ -1078,45 +1242,439 @@
         <v>1055</v>
       </c>
       <c r="H9" s="4">
-        <v>1040</v>
+        <v>1055</v>
       </c>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:12">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="5">
-        <f>B9-B8</f>
+        <f t="shared" ref="B10:H10" si="1">B9-B8</f>
         <v>30</v>
       </c>
       <c r="C10" s="5">
-        <f>C9-C8</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="D10" s="5">
-        <f>D9-D8</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="E10" s="5">
-        <f>E9-E8</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="F10" s="5">
-        <f>F9-F8</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="G10" s="5">
-        <f>G9-G8</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="H10" s="5">
-        <f>H9-H8</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="I10" s="5">
         <f>AVERAGE(B10:H10)</f>
         <v>29.571428571428573</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="15">
+        <v>0</v>
+      </c>
+      <c r="J13" s="15">
+        <v>0</v>
+      </c>
+      <c r="K13" s="15">
+        <v>0</v>
+      </c>
+      <c r="L13" s="8">
+        <f>AVERAGE(B13:K13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="15">
+        <v>1</v>
+      </c>
+      <c r="J14" s="15">
+        <v>1</v>
+      </c>
+      <c r="K14" s="15">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5">
+        <f>AVERAGE(B14:K14)</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="15">
+        <v>0</v>
+      </c>
+      <c r="J15" s="15">
+        <v>0</v>
+      </c>
+      <c r="K15" s="15">
+        <v>0</v>
+      </c>
+      <c r="L15" s="5">
+        <f>AVERAGE(B15:K15)</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="15">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="15">
+        <v>0</v>
+      </c>
+      <c r="J16" s="15">
+        <v>0</v>
+      </c>
+      <c r="K16" s="15">
+        <v>0</v>
+      </c>
+      <c r="L16" s="8">
+        <f>AVERAGE(B16:K16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="15">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="15">
+        <v>0</v>
+      </c>
+      <c r="J17" s="15">
+        <v>0</v>
+      </c>
+      <c r="K17" s="15">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5">
+        <f>AVERAGE(B17:K17)</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="15">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J18" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="K18" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="L18" s="5">
+        <f>AVERAGE(B18:K18)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="15">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="15">
+        <v>0</v>
+      </c>
+      <c r="J19" s="15">
+        <v>0</v>
+      </c>
+      <c r="K19" s="15">
+        <v>1</v>
+      </c>
+      <c r="L19" s="5">
+        <f>AVERAGE(B19:K19)</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="15">
+        <v>1010</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1010</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1010</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1010</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1010</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1010</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1010</v>
+      </c>
+      <c r="I20" s="15">
+        <v>1010</v>
+      </c>
+      <c r="J20" s="15">
+        <v>1010</v>
+      </c>
+      <c r="K20" s="15">
+        <v>1010</v>
+      </c>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1058</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1052</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1048</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1048</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1041</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1024</v>
+      </c>
+      <c r="H21" s="4">
+        <v>1029</v>
+      </c>
+      <c r="I21" s="15">
+        <v>1018</v>
+      </c>
+      <c r="J21" s="15">
+        <v>1039</v>
+      </c>
+      <c r="K21" s="15">
+        <v>1029</v>
+      </c>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="5">
+        <f t="shared" ref="B22" si="2">B21-B20</f>
+        <v>48</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" ref="C22" si="3">C21-C20</f>
+        <v>42</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" ref="D22" si="4">D21-D20</f>
+        <v>38</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" ref="E22" si="5">E21-E20</f>
+        <v>38</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" ref="F22" si="6">F21-F20</f>
+        <v>31</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" ref="G22" si="7">G21-G20</f>
+        <v>14</v>
+      </c>
+      <c r="H22" s="5">
+        <f t="shared" ref="H22:K22" si="8">H21-H20</f>
+        <v>19</v>
+      </c>
+      <c r="I22" s="5">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="J22" s="5">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+      <c r="L22" s="5">
+        <f>AVERAGE(B22:K22)</f>
+        <v>28.6</v>
       </c>
     </row>
   </sheetData>
@@ -1127,10 +1685,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L7"/>
+      <selection activeCell="B17" sqref="B17:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1176,7 +1734,7 @@
         <v>1</v>
       </c>
       <c r="M1" s="5">
-        <f>AVERAGE(B1:L1)</f>
+        <f t="shared" ref="M1:M7" si="0">AVERAGE(B1:L1)</f>
         <v>0.63636363636363635</v>
       </c>
       <c r="N1" s="2"/>
@@ -1220,7 +1778,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="5">
-        <f>AVERAGE(B2:L2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N2" s="2"/>
@@ -1264,7 +1822,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="8">
-        <f>AVERAGE(B3:L3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N3" s="2"/>
@@ -1308,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="8">
-        <f>AVERAGE(B4:L4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N4" s="2"/>
@@ -1352,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="5">
-        <f>AVERAGE(B5:L5)</f>
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
       <c r="N5" s="2"/>
@@ -1396,7 +1954,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="8">
-        <f>AVERAGE(B6:L6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N6" s="2"/>
@@ -1440,7 +1998,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="5">
-        <f>AVERAGE(B7:L7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N7" s="2"/>
@@ -1451,13 +2009,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>1015</v>
+        <v>1032</v>
       </c>
       <c r="C8" s="4">
         <v>1032</v>
       </c>
       <c r="D8" s="4">
-        <v>1016</v>
+        <v>1032</v>
       </c>
       <c r="E8" s="4">
         <v>1032</v>
@@ -1475,7 +2033,7 @@
         <v>1032</v>
       </c>
       <c r="J8" s="4">
-        <v>1015</v>
+        <v>1032</v>
       </c>
       <c r="K8" s="4">
         <v>1032</v>
@@ -1492,13 +2050,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="4">
-        <v>1040</v>
+        <v>1057</v>
       </c>
       <c r="C9" s="4">
         <v>1060</v>
       </c>
       <c r="D9" s="4">
-        <v>1045</v>
+        <v>1061</v>
       </c>
       <c r="E9" s="4">
         <v>1060</v>
@@ -1516,7 +2074,7 @@
         <v>1053</v>
       </c>
       <c r="J9" s="4">
-        <v>1043</v>
+        <v>1060</v>
       </c>
       <c r="K9" s="4">
         <v>1053</v>
@@ -1533,47 +2091,47 @@
         <v>9</v>
       </c>
       <c r="B10" s="5">
-        <f>B9-B8</f>
+        <f t="shared" ref="B10:L10" si="1">B9-B8</f>
         <v>25</v>
       </c>
       <c r="C10" s="5">
-        <f>C9-C8</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="D10" s="5">
-        <f>D9-D8</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="E10" s="5">
-        <f>E9-E8</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="F10" s="5">
-        <f>F9-F8</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="G10" s="5">
-        <f>G9-G8</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H10" s="5">
-        <f>H9-H8</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="I10" s="5">
-        <f>I9-I8</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="J10" s="5">
-        <f>J9-J8</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="K10" s="5">
-        <f>K9-K8</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="L10" s="5">
-        <f>L9-L8</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="M10" s="5">
@@ -1581,6 +2139,389 @@
         <v>24.181818181818183</v>
       </c>
       <c r="O10" s="1"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="15">
+        <v>1</v>
+      </c>
+      <c r="C13" s="15">
+        <v>0</v>
+      </c>
+      <c r="D13" s="15">
+        <v>1</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0</v>
+      </c>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
+      <c r="G13" s="16">
+        <v>0</v>
+      </c>
+      <c r="H13" s="16">
+        <v>0</v>
+      </c>
+      <c r="I13" s="16">
+        <v>0</v>
+      </c>
+      <c r="J13" s="16">
+        <v>0</v>
+      </c>
+      <c r="K13" s="18">
+        <f>AVERAGE(B13:J13)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L13" s="17"/>
+      <c r="M13" s="13"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="15">
+        <v>1</v>
+      </c>
+      <c r="C14" s="15">
+        <v>1</v>
+      </c>
+      <c r="D14" s="15">
+        <v>1</v>
+      </c>
+      <c r="E14" s="15">
+        <v>1</v>
+      </c>
+      <c r="F14" s="16">
+        <v>1</v>
+      </c>
+      <c r="G14" s="16">
+        <v>1</v>
+      </c>
+      <c r="H14" s="16">
+        <v>1</v>
+      </c>
+      <c r="I14" s="16">
+        <v>0</v>
+      </c>
+      <c r="J14" s="16">
+        <v>1</v>
+      </c>
+      <c r="K14" s="18">
+        <f>AVERAGE(B14:J14)</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="L14" s="17"/>
+      <c r="M14" s="13"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1</v>
+      </c>
+      <c r="G15" s="16">
+        <v>0</v>
+      </c>
+      <c r="H15" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="16">
+        <v>0</v>
+      </c>
+      <c r="J15" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="K15" s="18">
+        <f>AVERAGE(B15:J15)</f>
+        <v>0.25</v>
+      </c>
+      <c r="L15" s="17"/>
+      <c r="M15" s="13"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="15">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="15">
+        <v>0</v>
+      </c>
+      <c r="E16" s="15">
+        <v>0</v>
+      </c>
+      <c r="F16" s="16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="16">
+        <v>0</v>
+      </c>
+      <c r="H16" s="16">
+        <v>0</v>
+      </c>
+      <c r="I16" s="16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="16">
+        <v>0</v>
+      </c>
+      <c r="K16" s="18">
+        <f>AVERAGE(B16:J16)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="17"/>
+      <c r="M16" s="13"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="15">
+        <v>1</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1</v>
+      </c>
+      <c r="D17" s="15">
+        <v>1</v>
+      </c>
+      <c r="E17" s="15">
+        <v>0</v>
+      </c>
+      <c r="F17" s="16">
+        <v>1</v>
+      </c>
+      <c r="G17" s="16">
+        <v>0</v>
+      </c>
+      <c r="H17" s="16">
+        <v>1</v>
+      </c>
+      <c r="I17" s="16">
+        <v>0</v>
+      </c>
+      <c r="J17" s="16">
+        <v>1</v>
+      </c>
+      <c r="K17" s="18">
+        <f>AVERAGE(B17:J17)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L17" s="17"/>
+      <c r="M17" s="13"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="15">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="15">
+        <v>1</v>
+      </c>
+      <c r="E18" s="15">
+        <v>0</v>
+      </c>
+      <c r="F18" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="16">
+        <v>0</v>
+      </c>
+      <c r="H18" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="I18" s="16">
+        <v>0</v>
+      </c>
+      <c r="J18" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="K18" s="18">
+        <f>AVERAGE(B18:J18)</f>
+        <v>0.3125</v>
+      </c>
+      <c r="L18" s="17"/>
+      <c r="M18" s="13"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="15">
+        <v>1</v>
+      </c>
+      <c r="C19" s="15">
+        <v>0</v>
+      </c>
+      <c r="D19" s="15">
+        <v>0</v>
+      </c>
+      <c r="E19" s="15">
+        <v>1</v>
+      </c>
+      <c r="F19" s="16">
+        <v>0</v>
+      </c>
+      <c r="G19" s="16">
+        <v>1</v>
+      </c>
+      <c r="H19" s="16">
+        <v>0</v>
+      </c>
+      <c r="I19" s="16">
+        <v>1</v>
+      </c>
+      <c r="J19" s="16">
+        <v>1</v>
+      </c>
+      <c r="K19" s="18">
+        <f>AVERAGE(B19:J19)</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="L19" s="17"/>
+      <c r="M19" s="13"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="15">
+        <v>1015</v>
+      </c>
+      <c r="C20" s="15">
+        <v>1015</v>
+      </c>
+      <c r="D20" s="15">
+        <v>1015</v>
+      </c>
+      <c r="E20" s="15">
+        <v>1015</v>
+      </c>
+      <c r="F20" s="16">
+        <v>1015</v>
+      </c>
+      <c r="G20" s="16">
+        <v>1015</v>
+      </c>
+      <c r="H20" s="16">
+        <v>1015</v>
+      </c>
+      <c r="I20" s="16">
+        <v>1015</v>
+      </c>
+      <c r="J20" s="16">
+        <v>1015</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="13"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="15">
+        <v>1059</v>
+      </c>
+      <c r="C21" s="15">
+        <v>1050</v>
+      </c>
+      <c r="D21" s="15">
+        <v>1048</v>
+      </c>
+      <c r="E21" s="15">
+        <v>1045</v>
+      </c>
+      <c r="F21" s="16">
+        <v>1044</v>
+      </c>
+      <c r="G21" s="16">
+        <v>1041</v>
+      </c>
+      <c r="H21" s="16">
+        <v>1042</v>
+      </c>
+      <c r="I21" s="16">
+        <v>1035</v>
+      </c>
+      <c r="J21" s="16">
+        <v>1045</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="13"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="5">
+        <f t="shared" ref="B22" si="2">B21-B20</f>
+        <v>44</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" ref="C22" si="3">C21-C20</f>
+        <v>35</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" ref="D22" si="4">D21-D20</f>
+        <v>33</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" ref="E22" si="5">E21-E20</f>
+        <v>30</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" ref="F22" si="6">F21-F20</f>
+        <v>29</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" ref="G22" si="7">G21-G20</f>
+        <v>26</v>
+      </c>
+      <c r="H22" s="5">
+        <f t="shared" ref="H22" si="8">H21-H20</f>
+        <v>27</v>
+      </c>
+      <c r="I22" s="5">
+        <f t="shared" ref="I22:J22" si="9">I21-I20</f>
+        <v>20</v>
+      </c>
+      <c r="J22" s="5">
+        <f t="shared" si="9"/>
+        <v>30</v>
+      </c>
+      <c r="K22" s="5">
+        <f>AVERAGE(B22:I22)</f>
+        <v>30.5</v>
+      </c>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1590,29 +2531,35 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="2"/>
     <col min="4" max="4" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="16" t="s">
         <v>12</v>
       </c>
+      <c r="F1" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="G1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1620,42 +2567,48 @@
         <v>0</v>
       </c>
       <c r="B2" s="9">
+        <f>Without!I1</f>
         <v>0.14285714285714285</v>
       </c>
       <c r="C2" s="10">
+        <f>With!M1</f>
         <v>0.63636363636363635</v>
       </c>
       <c r="D2" s="10"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="9">
+        <f>Without!I2</f>
         <v>0.8571428571428571</v>
       </c>
       <c r="C3" s="10">
+        <f>With!M2</f>
         <v>1</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="9">
+        <f>Without!I3</f>
         <v>0.42857142857142855</v>
       </c>
       <c r="C4" s="10">
+        <f>With!M3</f>
         <v>0</v>
       </c>
       <c r="D4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="17">
+      <c r="F4" s="20"/>
+      <c r="G4" s="19">
         <v>4</v>
       </c>
     </row>
@@ -1664,34 +2617,38 @@
         <v>3</v>
       </c>
       <c r="B5" s="9">
+        <f>Without!I4</f>
         <v>0</v>
       </c>
       <c r="C5" s="10">
-        <v>0</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="18">
-        <v>1</v>
-      </c>
-      <c r="G5" s="10"/>
+        <f>With!M4</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="20">
+        <v>1</v>
+      </c>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="9">
+        <f>Without!I5</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="C6" s="10">
+        <f>With!M5</f>
         <v>0.125</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="F6" s="18">
-        <v>1</v>
-      </c>
-      <c r="G6" s="17">
+      <c r="F6" s="20">
+        <v>1</v>
+      </c>
+      <c r="G6" s="19">
         <v>3</v>
       </c>
     </row>
@@ -1700,14 +2657,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="9">
+        <f>Without!I6</f>
         <v>3.5714285714285712E-2</v>
       </c>
       <c r="C7" s="10">
+        <f>With!M6</f>
         <v>0</v>
       </c>
       <c r="D7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="17">
+      <c r="F7" s="20"/>
+      <c r="G7" s="19">
         <v>2</v>
       </c>
     </row>
@@ -1716,42 +2675,202 @@
         <v>6</v>
       </c>
       <c r="B8" s="9">
+        <f>Without!I7</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="C8" s="10">
+        <f>With!M7</f>
         <v>1</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="F8" s="18">
-        <v>1</v>
-      </c>
-      <c r="G8" s="17">
+      <c r="F8" s="20">
+        <v>1</v>
+      </c>
+      <c r="G8" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B9" s="9">
+        <f>Without!I10</f>
         <v>29.571428571428573</v>
       </c>
       <c r="C9" s="10">
+        <f>With!M10</f>
         <v>24.181818181818183</v>
       </c>
       <c r="D9" s="10"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="9">
+        <f>Without!L13</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="10">
+        <f>With!K13</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="19"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="9">
+        <f>Without!L14</f>
+        <v>0.9</v>
+      </c>
+      <c r="C14" s="10">
+        <f>With!K14</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="19"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="9">
+        <f>Without!L15</f>
+        <v>0.01</v>
+      </c>
+      <c r="C15" s="10">
+        <f>With!K15</f>
+        <v>0.25</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="9">
+        <f>Without!L16</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="10">
+        <f>With!K16</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="9">
+        <f>Without!L17</f>
+        <v>0.2</v>
+      </c>
+      <c r="C17" s="10">
+        <f>With!K17</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="19"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="9">
+        <f>Without!L18</f>
+        <v>0.25</v>
+      </c>
+      <c r="C18" s="10">
+        <f>With!K18</f>
+        <v>0.3125</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="9">
+        <f>Without!L19</f>
+        <v>0.4</v>
+      </c>
+      <c r="C19" s="10">
+        <f>With!K19</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="19"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="9">
+        <f>Without!L22</f>
+        <v>28.6</v>
+      </c>
+      <c r="C20" s="10">
+        <f>With!K22</f>
+        <v>30.5</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Results.xlsx by adding standard deviation
</commit_message>
<xml_diff>
--- a/Documents/Experimentos/02/Results.xlsx
+++ b/Documents/Experimentos/02/Results.xlsx
@@ -4,25 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Volunteers" sheetId="4" r:id="rId1"/>
     <sheet name="Without" sheetId="1" r:id="rId2"/>
     <sheet name="With" sheetId="2" r:id="rId3"/>
     <sheet name="Results" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="17" r:id="rId5"/>
-    <sheet name="Anova_Values" sheetId="5" r:id="rId6"/>
-    <sheet name="Anova_Results" sheetId="12" r:id="rId7"/>
-    <sheet name="Anova_All" sheetId="14" r:id="rId8"/>
-    <sheet name="Anova Example" sheetId="9" r:id="rId9"/>
+    <sheet name="Summary" sheetId="5" r:id="rId5"/>
+    <sheet name="Anova_Results" sheetId="12" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="105">
   <si>
     <t>Q3</t>
   </si>
@@ -258,30 +255,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>SSE: 10254</t>
-  </si>
-  <si>
-    <t>SSTR: 86049.55556</t>
-  </si>
-  <si>
-    <t>SST: 96303.55556</t>
-  </si>
-  <si>
-    <t>MSTR: 43024.78</t>
-  </si>
-  <si>
-    <t>MSE: 1709</t>
-  </si>
-  <si>
-    <t>df1: 2</t>
-  </si>
-  <si>
-    <t>df2: 6</t>
-  </si>
-  <si>
-    <t>Results (scale 0 to 10):</t>
-  </si>
-  <si>
     <t>Results(Scale 0 to 1):</t>
   </si>
   <si>
@@ -294,12 +267,6 @@
     <t>Q5: SUMMARY</t>
   </si>
   <si>
-    <t>Scale 0-1: SUMMARY</t>
-  </si>
-  <si>
-    <t>Scale 0-10: SUMMARY</t>
-  </si>
-  <si>
     <t>Q6: SUMMARY</t>
   </si>
   <si>
@@ -333,9 +300,6 @@
     <t>Reject this question</t>
   </si>
   <si>
-    <t>x10</t>
-  </si>
-  <si>
     <t>95% Confident they are Not Equal</t>
   </si>
   <si>
@@ -348,9 +312,6 @@
     <t>All Questions: SUMMARY</t>
   </si>
   <si>
-    <t>SUMMARY</t>
-  </si>
-  <si>
     <t>Equal number of correct answers</t>
   </si>
   <si>
@@ -367,13 +328,19 @@
   </si>
   <si>
     <t>alpha:</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,8 +369,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -488,6 +461,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -547,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -658,9 +637,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -670,6 +646,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3192,178 +3177,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:AA43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="29">
-        <v>16</v>
-      </c>
-      <c r="C5" s="29">
-        <v>3</v>
-      </c>
-      <c r="D5" s="29">
-        <v>0.1875</v>
-      </c>
-      <c r="E5" s="29">
-        <v>0.16250000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A6" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="30">
-        <v>16</v>
-      </c>
-      <c r="C6" s="30">
-        <v>3</v>
-      </c>
-      <c r="D6" s="30">
-        <v>0.1875</v>
-      </c>
-      <c r="E6" s="30">
-        <v>0.16250000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="29">
-        <v>0</v>
-      </c>
-      <c r="C11" s="29">
-        <v>1</v>
-      </c>
-      <c r="D11" s="29">
-        <v>0</v>
-      </c>
-      <c r="E11" s="29">
-        <v>0</v>
-      </c>
-      <c r="F11" s="29">
-        <v>1</v>
-      </c>
-      <c r="G11" s="29">
-        <v>4.1708767574426382</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="29">
-        <v>4.875</v>
-      </c>
-      <c r="C12" s="29">
-        <v>30</v>
-      </c>
-      <c r="D12" s="29">
-        <v>0.16250000000000001</v>
-      </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A14" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="30">
-        <v>4.875</v>
-      </c>
-      <c r="C14" s="30">
-        <v>31</v>
-      </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z47"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3380,7 +3197,10 @@
       <c r="A2" t="s">
         <v>56</v>
       </c>
-      <c r="S2" s="42" t="s">
+      <c r="R2" t="s">
+        <v>104</v>
+      </c>
+      <c r="S2" s="47" t="s">
         <v>103</v>
       </c>
       <c r="V2" t="s">
@@ -3443,9 +3263,9 @@
         <f t="shared" ref="R3:R9" si="0">AVERAGE(B3:Q3)</f>
         <v>0.5</v>
       </c>
-      <c r="S3" s="2">
-        <f t="shared" ref="S3:S9" si="1">R3 *10</f>
-        <v>5</v>
+      <c r="S3" s="48">
+        <f>STDEV(B3:Q3)</f>
+        <v>0.5163977794943222</v>
       </c>
       <c r="V3" s="3" t="s">
         <v>0</v>
@@ -3519,9 +3339,9 @@
         <f t="shared" si="0"/>
         <v>0.9375</v>
       </c>
-      <c r="S4" s="2">
-        <f t="shared" si="1"/>
-        <v>9.375</v>
+      <c r="S4" s="48">
+        <f>STDEV(B4:Q4)</f>
+        <v>0.25</v>
       </c>
       <c r="V4" s="3" t="s">
         <v>1</v>
@@ -3595,9 +3415,9 @@
         <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
-      <c r="S5" s="2">
-        <f t="shared" si="1"/>
-        <v>1.875</v>
+      <c r="S5" s="48">
+        <f>STDEV(B5:Q5)</f>
+        <v>0.40311288741492751</v>
       </c>
       <c r="V5" s="3" t="s">
         <v>2</v>
@@ -3671,8 +3491,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S6" s="2">
-        <f t="shared" si="1"/>
+      <c r="S6" s="48">
+        <f>STDEV(B6:Q6)</f>
         <v>0</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -3747,9 +3567,9 @@
         <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
-      <c r="S7" s="2">
-        <f t="shared" si="1"/>
-        <v>3.75</v>
+      <c r="S7" s="48">
+        <f>STDEV(B7:Q7)</f>
+        <v>0.5</v>
       </c>
       <c r="V7" s="3" t="s">
         <v>4</v>
@@ -3823,9 +3643,9 @@
         <f t="shared" si="0"/>
         <v>0.15625</v>
       </c>
-      <c r="S8" s="2">
-        <f t="shared" si="1"/>
-        <v>1.5625</v>
+      <c r="S8" s="48">
+        <f>STDEV(B8:Q8)</f>
+        <v>0.30103986446980741</v>
       </c>
       <c r="V8" s="3" t="s">
         <v>5</v>
@@ -3899,9 +3719,9 @@
         <f t="shared" si="0"/>
         <v>0.8125</v>
       </c>
-      <c r="S9" s="2">
-        <f t="shared" si="1"/>
-        <v>8.125</v>
+      <c r="S9" s="48">
+        <f>STDEV(B9:Q9)</f>
+        <v>0.40311288741492751</v>
       </c>
       <c r="V9" s="3" t="s">
         <v>6</v>
@@ -3972,7 +3792,7 @@
         <v>1015</v>
       </c>
       <c r="R10" s="25"/>
-      <c r="S10" s="2"/>
+      <c r="S10" s="49"/>
       <c r="V10" s="3" t="s">
         <v>7</v>
       </c>
@@ -4042,7 +3862,7 @@
         <v>1045</v>
       </c>
       <c r="R11" s="25"/>
-      <c r="S11" s="2"/>
+      <c r="S11" s="49"/>
       <c r="V11" s="3" t="s">
         <v>8</v>
       </c>
@@ -4064,74 +3884,77 @@
         <v>9</v>
       </c>
       <c r="B12" s="5">
-        <f t="shared" ref="B12:E12" si="2">B11-B10</f>
+        <f t="shared" ref="B12:E12" si="1">B11-B10</f>
         <v>25</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="D12" s="5">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" ref="F12:L12" si="2">C11-C10</f>
+        <v>18</v>
+      </c>
+      <c r="G12" s="5">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="E12" s="5">
+      <c r="H12" s="5">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="F12" s="5">
-        <f t="shared" ref="F12:L12" si="3">C11-C10</f>
-        <v>18</v>
-      </c>
-      <c r="G12" s="5">
+      <c r="I12" s="5">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="L12" s="5">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="M12" s="5">
+        <f t="shared" ref="M12:Q12" si="3">M11-M10</f>
+        <v>29</v>
+      </c>
+      <c r="N12" s="5">
         <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="H12" s="5">
+        <v>26</v>
+      </c>
+      <c r="O12" s="5">
         <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="I12" s="5">
+        <v>27</v>
+      </c>
+      <c r="P12" s="5">
         <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="J12" s="5">
+        <v>20</v>
+      </c>
+      <c r="Q12" s="5">
         <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="K12" s="5">
-        <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="L12" s="5">
-        <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="M12" s="5">
-        <f t="shared" ref="M12:Q12" si="4">M11-M10</f>
-        <v>29</v>
-      </c>
-      <c r="N12" s="5">
-        <f t="shared" si="4"/>
-        <v>26</v>
-      </c>
-      <c r="O12" s="5">
-        <f t="shared" si="4"/>
-        <v>27</v>
-      </c>
-      <c r="P12" s="5">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="Q12" s="5">
-        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="R12" s="25">
         <f>AVERAGE(B12:Q12)</f>
         <v>23.1875</v>
       </c>
-      <c r="S12" s="2"/>
+      <c r="S12" s="48">
+        <f>STDEV(B12:Q12)</f>
+        <v>4.2460766204422953</v>
+      </c>
       <c r="V12" s="3" t="s">
         <v>9</v>
       </c>
@@ -4215,12 +4038,12 @@
         <v>0</v>
       </c>
       <c r="R15" s="25">
-        <f t="shared" ref="R15:R21" si="5">AVERAGE(B15:Q15)</f>
+        <f t="shared" ref="R15:R21" si="4">AVERAGE(B15:Q15)</f>
         <v>6.25E-2</v>
       </c>
-      <c r="S15" s="2">
-        <f t="shared" ref="S15:S21" si="6">R15 *10</f>
-        <v>0.625</v>
+      <c r="S15" s="48">
+        <f>STDEV(B15:Q15)</f>
+        <v>0.25</v>
       </c>
       <c r="V15" s="3" t="s">
         <v>0</v>
@@ -4282,12 +4105,12 @@
         <v>0</v>
       </c>
       <c r="R16" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.875</v>
       </c>
-      <c r="S16" s="2">
-        <f t="shared" si="6"/>
-        <v>8.75</v>
+      <c r="S16" s="48">
+        <f>STDEV(B16:Q16)</f>
+        <v>0.34156502553198659</v>
       </c>
       <c r="V16" s="3" t="s">
         <v>1</v>
@@ -4296,7 +4119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:27">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -4349,12 +4172,12 @@
         <v>0</v>
       </c>
       <c r="R17" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.1875</v>
       </c>
-      <c r="S17" s="2">
-        <f t="shared" si="6"/>
-        <v>1.875</v>
+      <c r="S17" s="48">
+        <f>STDEV(B17:Q17)</f>
+        <v>0.40311288741492751</v>
       </c>
       <c r="V17" s="3" t="s">
         <v>2</v>
@@ -4363,7 +4186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:27">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
@@ -4416,11 +4239,11 @@
         <v>0</v>
       </c>
       <c r="R18" s="25">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S18" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S18" s="48">
+        <f>STDEV(B18:Q18)</f>
         <v>0</v>
       </c>
       <c r="V18" s="3" t="s">
@@ -4430,7 +4253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:27">
       <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
@@ -4483,12 +4306,12 @@
         <v>0</v>
       </c>
       <c r="R19" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
-      <c r="S19" s="2">
-        <f t="shared" si="6"/>
-        <v>2.5</v>
+      <c r="S19" s="48">
+        <f>STDEV(B19:Q19)</f>
+        <v>0.44721359549995793</v>
       </c>
       <c r="V19" s="3" t="s">
         <v>4</v>
@@ -4497,7 +4320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:27">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
@@ -4550,12 +4373,12 @@
         <v>0.5</v>
       </c>
       <c r="R20" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.171875</v>
       </c>
-      <c r="S20" s="2">
-        <f t="shared" si="6"/>
-        <v>1.71875</v>
+      <c r="S20" s="48">
+        <f>STDEV(B20:Q20)</f>
+        <v>0.2366211810750114</v>
       </c>
       <c r="V20" s="3" t="s">
         <v>5</v>
@@ -4564,7 +4387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:27">
       <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
@@ -4617,12 +4440,12 @@
         <v>1</v>
       </c>
       <c r="R21" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="S21" s="2">
-        <f t="shared" si="6"/>
-        <v>5</v>
+      <c r="S21" s="48">
+        <f>STDEV(B21:Q21)</f>
+        <v>0.5163977794943222</v>
       </c>
       <c r="V21" s="3" t="s">
         <v>6</v>
@@ -4631,7 +4454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:27">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -4684,6 +4507,7 @@
         <v>1010</v>
       </c>
       <c r="R22" s="25"/>
+      <c r="S22" s="49"/>
       <c r="V22" s="3" t="s">
         <v>7</v>
       </c>
@@ -4691,7 +4515,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:27">
       <c r="A23" s="3" t="s">
         <v>8</v>
       </c>
@@ -4744,6 +4568,7 @@
         <v>1029</v>
       </c>
       <c r="R23" s="25"/>
+      <c r="S23" s="49"/>
       <c r="V23" s="3" t="s">
         <v>8</v>
       </c>
@@ -4751,78 +4576,82 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:27">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="5">
-        <f t="shared" ref="B24:Q24" si="7">B23-B22</f>
+        <f t="shared" ref="B24:Q24" si="5">B23-B22</f>
         <v>20</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="D24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="E24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="F24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="G24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="H24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="I24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>42</v>
       </c>
       <c r="J24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>38</v>
       </c>
       <c r="K24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>38</v>
       </c>
       <c r="L24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="M24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="N24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="O24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="P24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="Q24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="R24" s="25">
         <f>AVERAGE(B24:Q24)</f>
         <v>28.9375</v>
       </c>
+      <c r="S24" s="48">
+        <f>STDEV(B24:Q24)</f>
+        <v>10.579658154527804</v>
+      </c>
       <c r="V24" s="3" t="s">
         <v>9</v>
       </c>
@@ -4831,1047 +4660,991 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:26">
-      <c r="D26" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" t="s">
-        <v>1</v>
-      </c>
-      <c r="J26" t="s">
+    <row r="26" spans="1:27">
+      <c r="E26" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
         <v>2</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>3</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>4</v>
       </c>
-      <c r="S26" t="s">
+      <c r="T26" t="s">
         <v>5</v>
       </c>
-      <c r="V26" t="s">
+      <c r="W26" t="s">
         <v>6</v>
       </c>
-      <c r="Y26" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26">
-      <c r="A27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="28" t="s">
+      <c r="Z26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27">
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="F27" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="G27" s="28" t="s">
+      <c r="H27" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="H27" s="28" t="s">
+      <c r="I27" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="J27" s="28" t="s">
+      <c r="K27" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="K27" s="28" t="s">
+      <c r="L27" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="M27" s="28" t="s">
+      <c r="N27" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="N27" s="28" t="s">
+      <c r="O27" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="P27" s="28" t="s">
+      <c r="Q27" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="Q27" s="28" t="s">
+      <c r="R27" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="S27" s="28" t="s">
+      <c r="T27" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="T27" s="28" t="s">
+      <c r="U27" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="V27" s="28" t="s">
+      <c r="W27" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="W27" s="28" t="s">
+      <c r="X27" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="Y27" s="28" t="s">
+      <c r="Z27" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="Z27" s="28" t="s">
+      <c r="AA27" s="28" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:26">
-      <c r="A28" s="28" t="s">
+    <row r="28" spans="1:27">
+      <c r="B28" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="C28" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="4">
-        <v>0</v>
-      </c>
       <c r="E28" s="4">
-        <v>1</v>
-      </c>
-      <c r="G28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
         <v>1</v>
       </c>
       <c r="H28" s="4">
         <v>1</v>
       </c>
-      <c r="J28" s="15">
-        <v>0</v>
-      </c>
-      <c r="K28" s="4">
-        <v>0</v>
-      </c>
-      <c r="M28" s="4">
+      <c r="I28" s="4">
+        <v>1</v>
+      </c>
+      <c r="K28" s="15">
+        <v>0</v>
+      </c>
+      <c r="L28" s="4">
         <v>0</v>
       </c>
       <c r="N28" s="4">
         <v>0</v>
       </c>
-      <c r="P28" s="4">
-        <v>1</v>
+      <c r="O28" s="4">
+        <v>0</v>
       </c>
       <c r="Q28" s="4">
         <v>1</v>
       </c>
-      <c r="S28" s="4">
-        <v>0</v>
+      <c r="R28" s="4">
+        <v>1</v>
       </c>
       <c r="T28" s="4">
         <v>0</v>
       </c>
-      <c r="V28" s="4">
-        <v>1</v>
+      <c r="U28" s="4">
+        <v>0</v>
       </c>
       <c r="W28" s="4">
         <v>1</v>
       </c>
-      <c r="Y28" s="4">
+      <c r="X28" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="4">
         <v>25</v>
       </c>
-      <c r="Z28" s="4">
+      <c r="AA28" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:26">
-      <c r="A29" s="4">
-        <f t="shared" ref="A29:A35" si="8">R3</f>
+    <row r="29" spans="1:27">
+      <c r="A29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="4">
+        <f t="shared" ref="B29:B35" si="6">R3</f>
         <v>0.5</v>
       </c>
-      <c r="B29" s="4">
-        <f t="shared" ref="B29:B35" si="9">R15</f>
+      <c r="C29" s="4">
+        <f t="shared" ref="C29:C35" si="7">R15</f>
         <v>6.25E-2</v>
       </c>
-      <c r="D29" s="6">
-        <v>1</v>
-      </c>
-      <c r="E29" s="4">
-        <v>0</v>
-      </c>
-      <c r="G29" s="6">
-        <v>1</v>
-      </c>
-      <c r="H29" s="4">
-        <v>1</v>
-      </c>
-      <c r="J29" s="6">
-        <v>0</v>
-      </c>
-      <c r="K29" s="4">
-        <v>1</v>
-      </c>
-      <c r="M29" s="6">
-        <v>0</v>
-      </c>
-      <c r="N29" s="4">
-        <v>0</v>
-      </c>
-      <c r="P29" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="4">
-        <v>0</v>
-      </c>
-      <c r="S29" s="6">
-        <v>0</v>
-      </c>
-      <c r="T29" s="4">
-        <v>0</v>
-      </c>
-      <c r="V29" s="6">
-        <v>1</v>
-      </c>
-      <c r="W29" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y29" s="4">
+      <c r="E29" s="6">
+        <v>1</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="6">
+        <v>1</v>
+      </c>
+      <c r="I29" s="4">
+        <v>1</v>
+      </c>
+      <c r="K29" s="6">
+        <v>0</v>
+      </c>
+      <c r="L29" s="4">
+        <v>1</v>
+      </c>
+      <c r="N29" s="6">
+        <v>0</v>
+      </c>
+      <c r="O29" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="6">
+        <v>0</v>
+      </c>
+      <c r="R29" s="4">
+        <v>0</v>
+      </c>
+      <c r="T29" s="6">
+        <v>0</v>
+      </c>
+      <c r="U29" s="4">
+        <v>0</v>
+      </c>
+      <c r="W29" s="6">
+        <v>1</v>
+      </c>
+      <c r="X29" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="4">
         <v>18</v>
       </c>
-      <c r="Z29" s="4">
+      <c r="AA29" s="4">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:26">
-      <c r="A30" s="4">
-        <f t="shared" si="8"/>
+    <row r="30" spans="1:27">
+      <c r="A30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" si="6"/>
         <v>0.9375</v>
       </c>
-      <c r="B30" s="4">
-        <f t="shared" si="9"/>
+      <c r="C30" s="4">
+        <f t="shared" si="7"/>
         <v>0.875</v>
       </c>
-      <c r="D30" s="6">
-        <v>1</v>
-      </c>
-      <c r="E30" s="4">
-        <v>0</v>
-      </c>
-      <c r="G30" s="6">
-        <v>1</v>
-      </c>
-      <c r="H30" s="4">
-        <v>1</v>
-      </c>
-      <c r="J30" s="6">
-        <v>0</v>
-      </c>
-      <c r="K30" s="4">
-        <v>1</v>
-      </c>
-      <c r="M30" s="6">
-        <v>0</v>
-      </c>
-      <c r="N30" s="4">
-        <v>0</v>
-      </c>
-      <c r="P30" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="4">
-        <v>1</v>
-      </c>
-      <c r="S30" s="6">
-        <v>0</v>
-      </c>
-      <c r="T30" s="4">
+      <c r="E30" s="6">
+        <v>1</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="H30" s="6">
+        <v>1</v>
+      </c>
+      <c r="I30" s="4">
+        <v>1</v>
+      </c>
+      <c r="K30" s="6">
+        <v>0</v>
+      </c>
+      <c r="L30" s="4">
+        <v>1</v>
+      </c>
+      <c r="N30" s="6">
+        <v>0</v>
+      </c>
+      <c r="O30" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="6">
+        <v>0</v>
+      </c>
+      <c r="R30" s="4">
+        <v>1</v>
+      </c>
+      <c r="T30" s="6">
+        <v>0</v>
+      </c>
+      <c r="U30" s="4">
         <v>0.25</v>
       </c>
-      <c r="V30" s="6">
-        <v>1</v>
-      </c>
-      <c r="W30" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y30" s="4">
+      <c r="W30" s="6">
+        <v>1</v>
+      </c>
+      <c r="X30" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="4">
         <v>19</v>
       </c>
-      <c r="Z30" s="4">
+      <c r="AA30" s="4">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:26">
-      <c r="A31" s="4">
-        <f t="shared" si="8"/>
+    <row r="31" spans="1:27">
+      <c r="A31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" si="6"/>
         <v>0.1875</v>
       </c>
-      <c r="B31" s="4">
-        <f t="shared" si="9"/>
+      <c r="C31" s="4">
+        <f t="shared" si="7"/>
         <v>0.1875</v>
       </c>
-      <c r="D31" s="6">
-        <v>1</v>
-      </c>
-      <c r="E31" s="4">
-        <v>0</v>
-      </c>
-      <c r="G31" s="6">
-        <v>1</v>
-      </c>
-      <c r="H31" s="4">
-        <v>1</v>
-      </c>
-      <c r="J31" s="6">
-        <v>0</v>
-      </c>
-      <c r="K31" s="4">
-        <v>1</v>
-      </c>
-      <c r="M31" s="6">
-        <v>0</v>
-      </c>
-      <c r="N31" s="4">
-        <v>0</v>
-      </c>
-      <c r="P31" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="4">
-        <v>0</v>
-      </c>
-      <c r="S31" s="6">
-        <v>0</v>
-      </c>
-      <c r="T31" s="4">
-        <v>0</v>
-      </c>
-      <c r="V31" s="6">
-        <v>1</v>
-      </c>
-      <c r="W31" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y31" s="4">
+      <c r="E31" s="6">
+        <v>1</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="H31" s="6">
+        <v>1</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1</v>
+      </c>
+      <c r="K31" s="6">
+        <v>0</v>
+      </c>
+      <c r="L31" s="4">
+        <v>1</v>
+      </c>
+      <c r="N31" s="6">
+        <v>0</v>
+      </c>
+      <c r="O31" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="6">
+        <v>0</v>
+      </c>
+      <c r="R31" s="4">
+        <v>0</v>
+      </c>
+      <c r="T31" s="6">
+        <v>0</v>
+      </c>
+      <c r="U31" s="4">
+        <v>0</v>
+      </c>
+      <c r="W31" s="6">
+        <v>1</v>
+      </c>
+      <c r="X31" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="4">
         <v>21</v>
       </c>
-      <c r="Z31" s="4">
+      <c r="AA31" s="4">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:26">
-      <c r="A32" s="4">
-        <f t="shared" si="8"/>
-        <v>0</v>
+    <row r="32" spans="1:27">
+      <c r="A32" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="B32" s="4">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="D32" s="6">
-        <v>1</v>
-      </c>
-      <c r="E32" s="4">
-        <v>0</v>
-      </c>
-      <c r="G32" s="6">
-        <v>1</v>
-      </c>
-      <c r="H32" s="4">
-        <v>1</v>
-      </c>
-      <c r="J32" s="6">
-        <v>0</v>
-      </c>
-      <c r="K32" s="4">
-        <v>0</v>
-      </c>
-      <c r="M32" s="6">
-        <v>0</v>
-      </c>
-      <c r="N32" s="4">
-        <v>0</v>
-      </c>
-      <c r="P32" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="4">
-        <v>0</v>
-      </c>
-      <c r="S32" s="6">
-        <v>0</v>
-      </c>
-      <c r="T32" s="4">
-        <v>0</v>
-      </c>
-      <c r="V32" s="6">
-        <v>1</v>
-      </c>
-      <c r="W32" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y32" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="6">
+        <v>1</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="H32" s="6">
+        <v>1</v>
+      </c>
+      <c r="I32" s="4">
+        <v>1</v>
+      </c>
+      <c r="K32" s="6">
+        <v>0</v>
+      </c>
+      <c r="L32" s="4">
+        <v>0</v>
+      </c>
+      <c r="N32" s="6">
+        <v>0</v>
+      </c>
+      <c r="O32" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="6">
+        <v>0</v>
+      </c>
+      <c r="R32" s="4">
+        <v>0</v>
+      </c>
+      <c r="T32" s="6">
+        <v>0</v>
+      </c>
+      <c r="U32" s="4">
+        <v>0</v>
+      </c>
+      <c r="W32" s="6">
+        <v>1</v>
+      </c>
+      <c r="X32" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z32" s="4">
         <v>18</v>
       </c>
-      <c r="Z32" s="4">
+      <c r="AA32" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:26">
-      <c r="A33" s="4">
-        <f t="shared" si="8"/>
+    <row r="33" spans="1:27">
+      <c r="A33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="4">
+        <f t="shared" si="6"/>
         <v>0.375</v>
       </c>
-      <c r="B33" s="4">
-        <f t="shared" si="9"/>
+      <c r="C33" s="4">
+        <f t="shared" si="7"/>
         <v>0.25</v>
       </c>
-      <c r="D33" s="6">
-        <v>0</v>
-      </c>
-      <c r="E33" s="4">
-        <v>0</v>
-      </c>
-      <c r="G33" s="6">
-        <v>1</v>
-      </c>
-      <c r="H33" s="4">
-        <v>0</v>
-      </c>
-      <c r="J33" s="6">
-        <v>0</v>
-      </c>
-      <c r="K33" s="4">
-        <v>0</v>
-      </c>
-      <c r="M33" s="6">
-        <v>0</v>
-      </c>
-      <c r="N33" s="4">
-        <v>0</v>
-      </c>
-      <c r="P33" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="4">
-        <v>0</v>
-      </c>
-      <c r="S33" s="6">
-        <v>0</v>
-      </c>
-      <c r="T33" s="4">
-        <v>0</v>
-      </c>
-      <c r="V33" s="6">
-        <v>1</v>
-      </c>
-      <c r="W33" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y33" s="4">
+      <c r="E33" s="6">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0</v>
+      </c>
+      <c r="H33" s="6">
+        <v>1</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0</v>
+      </c>
+      <c r="K33" s="6">
+        <v>0</v>
+      </c>
+      <c r="L33" s="4">
+        <v>0</v>
+      </c>
+      <c r="N33" s="6">
+        <v>0</v>
+      </c>
+      <c r="O33" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="6">
+        <v>0</v>
+      </c>
+      <c r="R33" s="4">
+        <v>0</v>
+      </c>
+      <c r="T33" s="6">
+        <v>0</v>
+      </c>
+      <c r="U33" s="4">
+        <v>0</v>
+      </c>
+      <c r="W33" s="6">
+        <v>1</v>
+      </c>
+      <c r="X33" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="4">
         <v>19</v>
       </c>
-      <c r="Z33" s="4">
+      <c r="AA33" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:26">
-      <c r="A34" s="4">
-        <f t="shared" si="8"/>
+    <row r="34" spans="1:27">
+      <c r="A34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="4">
+        <f t="shared" si="6"/>
         <v>0.15625</v>
       </c>
-      <c r="B34" s="4">
-        <f t="shared" si="9"/>
+      <c r="C34" s="4">
+        <f t="shared" si="7"/>
         <v>0.171875</v>
       </c>
-      <c r="D34" s="4">
-        <v>0</v>
-      </c>
       <c r="E34" s="4">
         <v>0</v>
       </c>
-      <c r="G34" s="4">
-        <v>1</v>
+      <c r="F34" s="4">
+        <v>0</v>
       </c>
       <c r="H34" s="4">
         <v>1</v>
       </c>
-      <c r="J34" s="4">
-        <v>0</v>
-      </c>
-      <c r="K34" s="15">
-        <v>0</v>
-      </c>
-      <c r="M34" s="4">
-        <v>0</v>
-      </c>
-      <c r="N34" s="15">
-        <v>0</v>
-      </c>
-      <c r="P34" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="15">
-        <v>0</v>
-      </c>
-      <c r="S34" s="4">
-        <v>0</v>
-      </c>
-      <c r="T34" s="15">
-        <v>0</v>
-      </c>
-      <c r="V34" s="4">
-        <v>1</v>
-      </c>
-      <c r="W34" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y34" s="4">
+      <c r="I34" s="4">
+        <v>1</v>
+      </c>
+      <c r="K34" s="4">
+        <v>0</v>
+      </c>
+      <c r="L34" s="15">
+        <v>0</v>
+      </c>
+      <c r="N34" s="4">
+        <v>0</v>
+      </c>
+      <c r="O34" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>0</v>
+      </c>
+      <c r="R34" s="15">
+        <v>0</v>
+      </c>
+      <c r="T34" s="4">
+        <v>0</v>
+      </c>
+      <c r="U34" s="15">
+        <v>0</v>
+      </c>
+      <c r="W34" s="4">
+        <v>1</v>
+      </c>
+      <c r="X34" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="4">
         <v>21</v>
       </c>
-      <c r="Z34" s="4">
+      <c r="AA34" s="4">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:26">
-      <c r="A35" s="4">
-        <f t="shared" si="8"/>
+    <row r="35" spans="1:27">
+      <c r="A35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="4">
+        <f t="shared" si="6"/>
         <v>0.8125</v>
       </c>
-      <c r="B35" s="4">
-        <f t="shared" si="9"/>
+      <c r="C35" s="4">
+        <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="D35" s="6">
-        <v>1</v>
-      </c>
-      <c r="E35" s="4">
-        <v>0</v>
-      </c>
-      <c r="G35" s="6">
-        <v>1</v>
-      </c>
-      <c r="H35" s="4">
-        <v>1</v>
-      </c>
-      <c r="J35" s="6">
-        <v>0</v>
-      </c>
-      <c r="K35" s="4">
-        <v>0</v>
-      </c>
-      <c r="M35" s="6">
-        <v>0</v>
-      </c>
-      <c r="N35" s="4">
-        <v>0</v>
-      </c>
-      <c r="P35" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="4">
-        <v>1</v>
-      </c>
-      <c r="S35" s="6">
-        <v>0</v>
-      </c>
-      <c r="T35" s="4">
-        <v>0</v>
-      </c>
-      <c r="V35" s="6">
-        <v>1</v>
-      </c>
-      <c r="W35" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y35" s="4">
+      <c r="E35" s="6">
+        <v>1</v>
+      </c>
+      <c r="F35" s="4">
+        <v>0</v>
+      </c>
+      <c r="H35" s="6">
+        <v>1</v>
+      </c>
+      <c r="I35" s="4">
+        <v>1</v>
+      </c>
+      <c r="K35" s="6">
+        <v>0</v>
+      </c>
+      <c r="L35" s="4">
+        <v>0</v>
+      </c>
+      <c r="N35" s="6">
+        <v>0</v>
+      </c>
+      <c r="O35" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="6">
+        <v>0</v>
+      </c>
+      <c r="R35" s="4">
+        <v>1</v>
+      </c>
+      <c r="T35" s="6">
+        <v>0</v>
+      </c>
+      <c r="U35" s="4">
+        <v>0</v>
+      </c>
+      <c r="W35" s="6">
+        <v>1</v>
+      </c>
+      <c r="X35" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z35" s="4">
         <v>21</v>
       </c>
-      <c r="Z35" s="4">
+      <c r="AA35" s="4">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:26">
-      <c r="A36" s="33">
+    <row r="36" spans="1:27">
+      <c r="A36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="33">
         <f>R12</f>
         <v>23.1875</v>
       </c>
-      <c r="B36" s="33">
+      <c r="C36" s="33">
         <f>R24</f>
         <v>28.9375</v>
       </c>
-      <c r="D36" s="15">
-        <v>1</v>
-      </c>
-      <c r="E36" s="4">
-        <v>0</v>
-      </c>
-      <c r="G36" s="15">
-        <v>1</v>
-      </c>
-      <c r="H36" s="4">
-        <v>1</v>
-      </c>
-      <c r="J36" s="15">
-        <v>0</v>
-      </c>
-      <c r="K36" s="4">
-        <v>0</v>
-      </c>
-      <c r="M36" s="15">
-        <v>0</v>
-      </c>
-      <c r="N36" s="4">
-        <v>0</v>
-      </c>
-      <c r="P36" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q36" s="4">
-        <v>0</v>
-      </c>
-      <c r="S36" s="15">
-        <v>0</v>
-      </c>
-      <c r="T36" s="4">
-        <v>0</v>
-      </c>
-      <c r="V36" s="15">
-        <v>1</v>
-      </c>
-      <c r="W36" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="4">
+      <c r="E36" s="15">
+        <v>1</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0</v>
+      </c>
+      <c r="H36" s="15">
+        <v>1</v>
+      </c>
+      <c r="I36" s="4">
+        <v>1</v>
+      </c>
+      <c r="K36" s="15">
+        <v>0</v>
+      </c>
+      <c r="L36" s="4">
+        <v>0</v>
+      </c>
+      <c r="N36" s="15">
+        <v>0</v>
+      </c>
+      <c r="O36" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="15">
+        <v>1</v>
+      </c>
+      <c r="R36" s="4">
+        <v>0</v>
+      </c>
+      <c r="T36" s="15">
+        <v>0</v>
+      </c>
+      <c r="U36" s="4">
+        <v>0</v>
+      </c>
+      <c r="W36" s="15">
+        <v>1</v>
+      </c>
+      <c r="X36" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="4">
         <v>28</v>
       </c>
-      <c r="Z36" s="4">
+      <c r="AA36" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:26">
-      <c r="D37" s="15">
-        <v>1</v>
-      </c>
-      <c r="E37" s="4">
-        <v>0</v>
-      </c>
-      <c r="G37" s="15">
-        <v>1</v>
-      </c>
-      <c r="H37" s="4">
-        <v>1</v>
-      </c>
-      <c r="J37" s="15">
-        <v>0</v>
-      </c>
-      <c r="K37" s="4">
-        <v>0</v>
-      </c>
-      <c r="M37" s="15">
-        <v>0</v>
-      </c>
-      <c r="N37" s="4">
-        <v>0</v>
-      </c>
-      <c r="P37" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="4">
-        <v>1</v>
-      </c>
-      <c r="S37" s="15">
-        <v>1</v>
-      </c>
-      <c r="T37" s="4">
-        <v>0</v>
-      </c>
-      <c r="V37" s="15">
-        <v>0</v>
-      </c>
-      <c r="W37" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y37" s="4">
+    <row r="37" spans="1:27">
+      <c r="E37" s="15">
+        <v>1</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0</v>
+      </c>
+      <c r="H37" s="15">
+        <v>1</v>
+      </c>
+      <c r="I37" s="4">
+        <v>1</v>
+      </c>
+      <c r="K37" s="15">
+        <v>0</v>
+      </c>
+      <c r="L37" s="4">
+        <v>0</v>
+      </c>
+      <c r="N37" s="15">
+        <v>0</v>
+      </c>
+      <c r="O37" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="15">
+        <v>1</v>
+      </c>
+      <c r="R37" s="4">
+        <v>1</v>
+      </c>
+      <c r="T37" s="15">
+        <v>1</v>
+      </c>
+      <c r="U37" s="4">
+        <v>0</v>
+      </c>
+      <c r="W37" s="15">
+        <v>0</v>
+      </c>
+      <c r="X37" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z37" s="4">
         <v>21</v>
       </c>
-      <c r="Z37" s="4">
+      <c r="AA37" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:26">
-      <c r="A38" t="s">
-        <v>85</v>
-      </c>
-      <c r="D38" s="15">
-        <v>0</v>
-      </c>
-      <c r="E38" s="4">
-        <v>0</v>
-      </c>
-      <c r="G38" s="15">
-        <v>1</v>
-      </c>
-      <c r="H38" s="4">
-        <v>1</v>
-      </c>
-      <c r="J38" s="15">
-        <v>0</v>
-      </c>
-      <c r="K38" s="4">
-        <v>0</v>
-      </c>
-      <c r="M38" s="15">
-        <v>0</v>
-      </c>
-      <c r="N38" s="4">
-        <v>0</v>
-      </c>
-      <c r="P38" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="4">
-        <v>0</v>
-      </c>
-      <c r="S38" s="15">
-        <v>0</v>
-      </c>
-      <c r="T38" s="4">
+    <row r="38" spans="1:27">
+      <c r="E38" s="15">
+        <v>0</v>
+      </c>
+      <c r="F38" s="4">
+        <v>0</v>
+      </c>
+      <c r="H38" s="15">
+        <v>1</v>
+      </c>
+      <c r="I38" s="4">
+        <v>1</v>
+      </c>
+      <c r="K38" s="15">
+        <v>0</v>
+      </c>
+      <c r="L38" s="4">
+        <v>0</v>
+      </c>
+      <c r="N38" s="15">
+        <v>0</v>
+      </c>
+      <c r="O38" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="15">
+        <v>0</v>
+      </c>
+      <c r="R38" s="4">
+        <v>0</v>
+      </c>
+      <c r="T38" s="15">
+        <v>0</v>
+      </c>
+      <c r="U38" s="4">
         <v>0.5</v>
       </c>
-      <c r="V38" s="15">
-        <v>1</v>
-      </c>
-      <c r="W38" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y38" s="4">
+      <c r="W38" s="15">
+        <v>1</v>
+      </c>
+      <c r="X38" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z38" s="4">
         <v>28</v>
       </c>
-      <c r="Z38" s="4">
+      <c r="AA38" s="4">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:26">
-      <c r="A39" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" s="16">
-        <v>1</v>
-      </c>
-      <c r="E39" s="4">
-        <v>0</v>
-      </c>
-      <c r="G39" s="16">
-        <v>1</v>
-      </c>
-      <c r="H39" s="4">
-        <v>1</v>
-      </c>
-      <c r="J39" s="16">
-        <v>1</v>
-      </c>
-      <c r="K39" s="4">
-        <v>0</v>
-      </c>
-      <c r="M39" s="16">
-        <v>0</v>
-      </c>
-      <c r="N39" s="4">
-        <v>0</v>
-      </c>
-      <c r="P39" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q39" s="4">
-        <v>0</v>
-      </c>
-      <c r="S39" s="16">
+    <row r="39" spans="1:27">
+      <c r="E39" s="16">
+        <v>1</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0</v>
+      </c>
+      <c r="H39" s="16">
+        <v>1</v>
+      </c>
+      <c r="I39" s="4">
+        <v>1</v>
+      </c>
+      <c r="K39" s="16">
+        <v>1</v>
+      </c>
+      <c r="L39" s="4">
+        <v>0</v>
+      </c>
+      <c r="N39" s="16">
+        <v>0</v>
+      </c>
+      <c r="O39" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="16">
+        <v>1</v>
+      </c>
+      <c r="R39" s="4">
+        <v>0</v>
+      </c>
+      <c r="T39" s="16">
         <v>0.5</v>
       </c>
-      <c r="T39" s="4">
+      <c r="U39" s="4">
         <v>0.5</v>
       </c>
-      <c r="V39" s="16">
-        <v>0</v>
-      </c>
-      <c r="W39" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y39" s="4">
+      <c r="W39" s="16">
+        <v>0</v>
+      </c>
+      <c r="X39" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="4">
         <v>29</v>
       </c>
-      <c r="Z39" s="4">
+      <c r="AA39" s="4">
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:26">
-      <c r="A40" s="4">
-        <f t="shared" ref="A40:A46" si="10">S3</f>
-        <v>5</v>
-      </c>
-      <c r="B40" s="4">
-        <f t="shared" ref="B40:B46" si="11">S15</f>
-        <v>0.625</v>
-      </c>
-      <c r="D40" s="16">
-        <v>0</v>
-      </c>
-      <c r="E40" s="4">
-        <v>0</v>
-      </c>
-      <c r="G40" s="16">
-        <v>1</v>
-      </c>
-      <c r="H40" s="4">
-        <v>1</v>
-      </c>
-      <c r="J40" s="16">
-        <v>0</v>
-      </c>
-      <c r="K40" s="4">
-        <v>0</v>
-      </c>
-      <c r="M40" s="16">
-        <v>0</v>
-      </c>
-      <c r="N40" s="4">
-        <v>0</v>
-      </c>
-      <c r="P40" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="4">
-        <v>0</v>
-      </c>
-      <c r="S40" s="16">
-        <v>0</v>
-      </c>
-      <c r="T40" s="4">
-        <v>0</v>
-      </c>
-      <c r="V40" s="16">
-        <v>1</v>
-      </c>
-      <c r="W40" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y40" s="4">
+    <row r="40" spans="1:27">
+      <c r="E40" s="16">
+        <v>0</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0</v>
+      </c>
+      <c r="H40" s="16">
+        <v>1</v>
+      </c>
+      <c r="I40" s="4">
+        <v>1</v>
+      </c>
+      <c r="K40" s="16">
+        <v>0</v>
+      </c>
+      <c r="L40" s="4">
+        <v>0</v>
+      </c>
+      <c r="N40" s="16">
+        <v>0</v>
+      </c>
+      <c r="O40" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="16">
+        <v>0</v>
+      </c>
+      <c r="R40" s="4">
+        <v>0</v>
+      </c>
+      <c r="T40" s="16">
+        <v>0</v>
+      </c>
+      <c r="U40" s="4">
+        <v>0</v>
+      </c>
+      <c r="W40" s="16">
+        <v>1</v>
+      </c>
+      <c r="X40" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="4">
         <v>26</v>
       </c>
-      <c r="Z40" s="4">
+      <c r="AA40" s="4">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:26">
-      <c r="A41" s="4">
-        <f t="shared" si="10"/>
-        <v>9.375</v>
-      </c>
-      <c r="B41" s="4">
-        <f t="shared" si="11"/>
-        <v>8.75</v>
-      </c>
-      <c r="D41" s="16">
-        <v>0</v>
-      </c>
-      <c r="E41" s="15">
-        <v>0</v>
-      </c>
-      <c r="G41" s="16">
-        <v>1</v>
-      </c>
-      <c r="H41" s="15">
-        <v>1</v>
-      </c>
-      <c r="J41" s="23">
-        <v>1</v>
-      </c>
-      <c r="K41" s="15">
-        <v>0</v>
-      </c>
-      <c r="M41" s="16">
-        <v>0</v>
-      </c>
-      <c r="N41" s="15">
-        <v>0</v>
-      </c>
-      <c r="P41" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q41" s="15">
-        <v>0</v>
-      </c>
-      <c r="S41" s="16">
+    <row r="41" spans="1:27">
+      <c r="E41" s="16">
+        <v>0</v>
+      </c>
+      <c r="F41" s="15">
+        <v>0</v>
+      </c>
+      <c r="H41" s="16">
+        <v>1</v>
+      </c>
+      <c r="I41" s="15">
+        <v>1</v>
+      </c>
+      <c r="K41" s="23">
+        <v>1</v>
+      </c>
+      <c r="L41" s="15">
+        <v>0</v>
+      </c>
+      <c r="N41" s="16">
+        <v>0</v>
+      </c>
+      <c r="O41" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="16">
+        <v>1</v>
+      </c>
+      <c r="R41" s="15">
+        <v>0</v>
+      </c>
+      <c r="T41" s="16">
         <v>0.5</v>
       </c>
-      <c r="T41" s="15">
+      <c r="U41" s="15">
         <v>0.5</v>
       </c>
-      <c r="V41" s="16">
-        <v>0</v>
-      </c>
-      <c r="W41" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y41" s="4">
+      <c r="W41" s="16">
+        <v>0</v>
+      </c>
+      <c r="X41" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="4">
         <v>27</v>
       </c>
-      <c r="Z41" s="4">
+      <c r="AA41" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:26">
-      <c r="A42" s="4">
-        <f t="shared" si="10"/>
-        <v>1.875</v>
-      </c>
-      <c r="B42" s="4">
-        <f t="shared" si="11"/>
-        <v>1.875</v>
-      </c>
-      <c r="D42" s="16">
-        <v>0</v>
-      </c>
-      <c r="E42" s="15">
-        <v>0</v>
-      </c>
-      <c r="G42" s="16">
-        <v>0</v>
-      </c>
-      <c r="H42" s="15">
-        <v>1</v>
-      </c>
-      <c r="J42" s="16">
-        <v>0</v>
-      </c>
-      <c r="K42" s="15">
-        <v>0</v>
-      </c>
-      <c r="M42" s="16">
-        <v>0</v>
-      </c>
-      <c r="N42" s="15">
-        <v>0</v>
-      </c>
-      <c r="P42" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="15">
-        <v>0</v>
-      </c>
-      <c r="S42" s="16">
-        <v>0</v>
-      </c>
-      <c r="T42" s="15">
+    <row r="42" spans="1:27">
+      <c r="E42" s="16">
+        <v>0</v>
+      </c>
+      <c r="F42" s="15">
+        <v>0</v>
+      </c>
+      <c r="H42" s="16">
+        <v>0</v>
+      </c>
+      <c r="I42" s="15">
+        <v>1</v>
+      </c>
+      <c r="K42" s="16">
+        <v>0</v>
+      </c>
+      <c r="L42" s="15">
+        <v>0</v>
+      </c>
+      <c r="N42" s="16">
+        <v>0</v>
+      </c>
+      <c r="O42" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="16">
+        <v>0</v>
+      </c>
+      <c r="R42" s="15">
+        <v>0</v>
+      </c>
+      <c r="T42" s="16">
+        <v>0</v>
+      </c>
+      <c r="U42" s="15">
         <v>0.5</v>
       </c>
-      <c r="V42" s="16">
-        <v>1</v>
-      </c>
-      <c r="W42" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y42" s="4">
+      <c r="W42" s="16">
+        <v>1</v>
+      </c>
+      <c r="X42" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="4">
         <v>20</v>
       </c>
-      <c r="Z42" s="4">
+      <c r="AA42" s="4">
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:26">
-      <c r="A43" s="4">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="B43" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="D43" s="16">
-        <v>0</v>
-      </c>
-      <c r="E43" s="15">
-        <v>0</v>
-      </c>
-      <c r="G43" s="16">
-        <v>1</v>
-      </c>
-      <c r="H43" s="15">
-        <v>0</v>
-      </c>
-      <c r="J43" s="23">
-        <v>1</v>
-      </c>
-      <c r="K43" s="15">
-        <v>0</v>
-      </c>
-      <c r="M43" s="16">
-        <v>0</v>
-      </c>
-      <c r="N43" s="15">
-        <v>0</v>
-      </c>
-      <c r="P43" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q43" s="15">
-        <v>0</v>
-      </c>
-      <c r="S43" s="16">
+    <row r="43" spans="1:27">
+      <c r="E43" s="16">
+        <v>0</v>
+      </c>
+      <c r="F43" s="15">
+        <v>0</v>
+      </c>
+      <c r="H43" s="16">
+        <v>1</v>
+      </c>
+      <c r="I43" s="15">
+        <v>0</v>
+      </c>
+      <c r="K43" s="23">
+        <v>1</v>
+      </c>
+      <c r="L43" s="15">
+        <v>0</v>
+      </c>
+      <c r="N43" s="16">
+        <v>0</v>
+      </c>
+      <c r="O43" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="16">
+        <v>1</v>
+      </c>
+      <c r="R43" s="15">
+        <v>0</v>
+      </c>
+      <c r="T43" s="16">
         <v>0.5</v>
       </c>
-      <c r="T43" s="15">
+      <c r="U43" s="15">
         <v>0.5</v>
       </c>
-      <c r="V43" s="16">
-        <v>1</v>
-      </c>
-      <c r="W43" s="15">
-        <v>1</v>
-      </c>
-      <c r="Y43" s="4">
+      <c r="W43" s="16">
+        <v>1</v>
+      </c>
+      <c r="X43" s="15">
+        <v>1</v>
+      </c>
+      <c r="Z43" s="4">
         <v>30</v>
       </c>
-      <c r="Z43" s="4">
+      <c r="AA43" s="4">
         <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:26">
-      <c r="A44" s="4">
-        <f t="shared" si="10"/>
-        <v>3.75</v>
-      </c>
-      <c r="B44" s="4">
-        <f t="shared" si="11"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:26">
-      <c r="A45" s="4">
-        <f t="shared" si="10"/>
-        <v>1.5625</v>
-      </c>
-      <c r="B45" s="4">
-        <f t="shared" si="11"/>
-        <v>1.71875</v>
-      </c>
-    </row>
-    <row r="46" spans="1:26">
-      <c r="A46" s="4">
-        <f t="shared" si="10"/>
-        <v>8.125</v>
-      </c>
-      <c r="B46" s="4">
-        <f t="shared" si="11"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:26">
-      <c r="A47" s="33">
-        <f>R12</f>
-        <v>23.1875</v>
-      </c>
-      <c r="B47" s="33">
-        <f>R24</f>
-        <v>28.9375</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5893,7 +5666,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="34" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
@@ -5903,7 +5676,7 @@
       <c r="G3" s="34"/>
       <c r="H3" s="2"/>
       <c r="I3" s="34" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="J3" s="34"/>
       <c r="K3" s="34"/>
@@ -6266,7 +6039,7 @@
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1">
       <c r="A16" s="34" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
@@ -6276,7 +6049,7 @@
       <c r="G16" s="34"/>
       <c r="H16" s="2"/>
       <c r="I16" s="34" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
@@ -6639,10 +6412,10 @@
     </row>
     <row r="29" spans="1:15" ht="15.75" thickBot="1">
       <c r="A29" s="39" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B29" s="40" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
@@ -6651,7 +6424,7 @@
       <c r="G29" s="39"/>
       <c r="H29" s="2"/>
       <c r="I29" s="34" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J29" s="34"/>
       <c r="K29" s="34"/>
@@ -6704,7 +6477,7 @@
       <c r="B31" s="13">
         <v>16</v>
       </c>
-      <c r="C31" s="45">
+      <c r="C31" s="44">
         <v>3</v>
       </c>
       <c r="D31" s="13">
@@ -6741,7 +6514,7 @@
       <c r="B32" s="32">
         <v>16</v>
       </c>
-      <c r="C32" s="46">
+      <c r="C32" s="45">
         <v>3</v>
       </c>
       <c r="D32" s="32">
@@ -7014,21 +6787,21 @@
     </row>
     <row r="42" spans="1:15" ht="15.75" thickBot="1">
       <c r="A42" s="39" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B42" s="40" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C42" s="39"/>
       <c r="D42" s="39"/>
       <c r="E42" s="39" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="F42" s="39"/>
       <c r="G42" s="39"/>
       <c r="H42" s="2"/>
       <c r="I42" s="24" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="J42" s="24"/>
       <c r="K42" s="24"/>
@@ -7079,7 +6852,7 @@
       <c r="B44" s="13">
         <v>16</v>
       </c>
-      <c r="C44" s="45">
+      <c r="C44" s="44">
         <v>0</v>
       </c>
       <c r="D44" s="13">
@@ -7114,7 +6887,7 @@
       <c r="B45" s="32">
         <v>16</v>
       </c>
-      <c r="C45" s="46">
+      <c r="C45" s="45">
         <v>0</v>
       </c>
       <c r="D45" s="32">
@@ -7257,7 +7030,7 @@
       <c r="L50" s="29">
         <v>5.1987304687500346E-2</v>
       </c>
-      <c r="M50" s="43">
+      <c r="M50" s="42">
         <v>0.47620639934230602</v>
       </c>
       <c r="N50" s="29">
@@ -7348,30 +7121,30 @@
     </row>
     <row r="55" spans="1:15" ht="15.75" thickBot="1">
       <c r="A55" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="B55" s="47">
+        <v>102</v>
+      </c>
+      <c r="B55" s="46">
         <v>0.05</v>
       </c>
-      <c r="I55" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="J55" s="44"/>
-      <c r="K55" s="44"/>
-      <c r="L55" s="44"/>
-      <c r="M55" s="44"/>
-      <c r="N55" s="44"/>
-      <c r="O55" s="44"/>
+      <c r="I55" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="J55" s="43"/>
+      <c r="K55" s="43"/>
+      <c r="L55" s="43"/>
+      <c r="M55" s="43"/>
+      <c r="N55" s="43"/>
+      <c r="O55" s="43"/>
     </row>
     <row r="56" spans="1:15">
       <c r="A56" s="36" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C56" s="37" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="I56" s="31" t="s">
         <v>62</v>
@@ -7391,13 +7164,13 @@
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="35" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C57" s="35" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="I57" s="29" t="s">
         <v>59</v>
@@ -7434,18 +7207,18 @@
     </row>
     <row r="59" spans="1:15">
       <c r="A59" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:15">
       <c r="A60" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="15.75" thickBot="1">
@@ -7489,7 +7262,7 @@
       <c r="L63" s="29">
         <v>264.5</v>
       </c>
-      <c r="M63" s="43">
+      <c r="M63" s="42">
         <v>4.0705354280218016</v>
       </c>
       <c r="N63" s="29">
@@ -7543,427 +7316,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="29">
-        <v>7</v>
-      </c>
-      <c r="C5" s="29">
-        <v>2.90625</v>
-      </c>
-      <c r="D5" s="29">
-        <v>0.41517857142857145</v>
-      </c>
-      <c r="E5" s="29">
-        <v>0.12718563988095236</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A6" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="30">
-        <v>7</v>
-      </c>
-      <c r="C6" s="30">
-        <v>2.0531250000000001</v>
-      </c>
-      <c r="D6" s="30">
-        <v>0.29330357142857144</v>
-      </c>
-      <c r="E6" s="30">
-        <v>9.1153738839285695E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="29">
-        <v>5.1987304687500346E-2</v>
-      </c>
-      <c r="C11" s="29">
-        <v>1</v>
-      </c>
-      <c r="D11" s="29">
-        <v>5.1987304687500346E-2</v>
-      </c>
-      <c r="E11" s="29">
-        <v>0.47620639934230602</v>
-      </c>
-      <c r="F11" s="29">
-        <v>0.50327382776323215</v>
-      </c>
-      <c r="G11" s="29">
-        <v>4.7472253358190439</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="29">
-        <v>1.3100362723214285</v>
-      </c>
-      <c r="C12" s="29">
-        <v>12</v>
-      </c>
-      <c r="D12" s="29">
-        <v>0.10916968936011905</v>
-      </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A14" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="30">
-        <v>1.3620235770089288</v>
-      </c>
-      <c r="C14" s="30">
-        <v>13</v>
-      </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="13">
-        <v>7</v>
-      </c>
-      <c r="C19" s="13">
-        <v>29.145833333333336</v>
-      </c>
-      <c r="D19" s="13">
-        <v>4.1636904761904763</v>
-      </c>
-      <c r="E19" s="13">
-        <v>12.638950892857139</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A20" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="32">
-        <v>7</v>
-      </c>
-      <c r="C20" s="32">
-        <v>20.53125</v>
-      </c>
-      <c r="D20" s="32">
-        <v>2.9330357142857144</v>
-      </c>
-      <c r="E20" s="32">
-        <v>9.1153738839285712</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" s="31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="13">
-        <v>5.3007890004960529</v>
-      </c>
-      <c r="C25" s="13">
-        <v>1</v>
-      </c>
-      <c r="D25" s="13">
-        <v>5.3007890004960529</v>
-      </c>
-      <c r="E25" s="13">
-        <v>0.48733197236740583</v>
-      </c>
-      <c r="F25" s="13">
-        <v>0.49842463965141615</v>
-      </c>
-      <c r="G25" s="13">
-        <v>4.7472253358190439</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" s="13">
-        <v>130.52594866071428</v>
-      </c>
-      <c r="C26" s="13">
-        <v>12</v>
-      </c>
-      <c r="D26" s="13">
-        <v>10.877162388392856</v>
-      </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A28" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="32">
-        <v>135.82673766121033</v>
-      </c>
-      <c r="C28" s="32">
-        <v>13</v>
-      </c>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="2">
-        <v>25.175409999999999</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.207E-3</v>
-      </c>
-      <c r="G3" s="2">
-        <v>5.143249</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="2">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated table by adding normality test results and wilcoxon's Added boxplot graphs
</commit_message>
<xml_diff>
--- a/Documents/Experimentos/02/Results.xlsx
+++ b/Documents/Experimentos/02/Results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="63">
   <si>
     <t>Q3</t>
   </si>
@@ -182,13 +182,37 @@
   </si>
   <si>
     <t>Timeout</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>&lt; 0.001</t>
+  </si>
+  <si>
+    <t>Wilcoxon Test</t>
+  </si>
+  <si>
+    <t>Boxplot</t>
+  </si>
+  <si>
+    <t>α = 0.05</t>
+  </si>
+  <si>
+    <t>Normality: Shapiro-Wilk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,8 +240,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,8 +334,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4F81BD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA7BFDE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD3DFEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -314,11 +376,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -387,6 +462,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,6 +493,106 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>616323</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>89648</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>560293</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>123266</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="616323" y="9805148"/>
+          <a:ext cx="7866529" cy="4796118"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>41462</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>108137</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9155206" y="9547412"/>
+          <a:ext cx="1229285" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2563,16 +2762,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:AA43"/>
+  <dimension ref="A2:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O59" sqref="O59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:26">
@@ -5037,8 +5237,197 @@
         <v>19</v>
       </c>
     </row>
+    <row r="46" spans="1:27">
+      <c r="B46" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="34"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="L46" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="M46" s="25"/>
+    </row>
+    <row r="47" spans="1:27">
+      <c r="B47" s="28"/>
+      <c r="C47" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="H47" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I47" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="J47" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="L47" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="M47" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="N47" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="O47" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="P47" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q47" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="R47" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="S47" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="T47" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27">
+      <c r="B48" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="29">
+        <v>4.3399999999999998E-5</v>
+      </c>
+      <c r="D48" s="29">
+        <v>4.5529999999999998E-8</v>
+      </c>
+      <c r="E48" s="29">
+        <v>1.5749999999999999E-8</v>
+      </c>
+      <c r="F48" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="G48" s="29">
+        <v>2.5660000000000002E-5</v>
+      </c>
+      <c r="H48" s="29">
+        <v>1.2130000000000001E-5</v>
+      </c>
+      <c r="I48" s="29">
+        <v>1.575E-6</v>
+      </c>
+      <c r="J48" s="30">
+        <v>4.3369999999999999E-2</v>
+      </c>
+      <c r="L48" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="M48" s="30">
+        <v>7.2589999999999998E-3</v>
+      </c>
+      <c r="N48" s="30">
+        <v>0.57569999999999999</v>
+      </c>
+      <c r="O48" s="30">
+        <v>1</v>
+      </c>
+      <c r="P48" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q48" s="30">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="R48" s="30">
+        <v>0.60980000000000001</v>
+      </c>
+      <c r="S48" s="30">
+        <v>7.0489999999999997E-2</v>
+      </c>
+      <c r="T48" s="30">
+        <v>3.5950000000000003E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:20">
+      <c r="B49" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="31">
+        <v>4.5529999999999998E-8</v>
+      </c>
+      <c r="D49" s="31">
+        <v>3.4079999999999998E-7</v>
+      </c>
+      <c r="E49" s="31">
+        <v>1.575E-6</v>
+      </c>
+      <c r="F49" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G49" s="31">
+        <v>5.2719999999999997E-6</v>
+      </c>
+      <c r="H49" s="31">
+        <v>4.778E-5</v>
+      </c>
+      <c r="I49" s="31">
+        <v>4.3399999999999998E-5</v>
+      </c>
+      <c r="J49" s="32">
+        <v>0.73629999999999995</v>
+      </c>
+      <c r="L49" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="M49" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="N49" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="O49" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="P49" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q49" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="R49" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="S49" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="T49" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="2:20">
+      <c r="B51" s="35" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed layout of Results.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Experimentos/02/Results.xlsx
+++ b/Documents/Experimentos/02/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Volunteers" sheetId="4" r:id="rId1"/>
@@ -1204,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1377,7 +1377,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="4">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="I6" s="5">
         <f t="shared" si="0"/>
-        <v>3.5714285714285712E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -2764,8 +2764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O59" sqref="O59"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3934,8 +3934,8 @@
       <c r="C20" s="4">
         <v>0</v>
       </c>
-      <c r="D20" s="4">
-        <v>0.25</v>
+      <c r="D20" s="12">
+        <v>0</v>
       </c>
       <c r="E20" s="4">
         <v>0</v>
@@ -3978,11 +3978,11 @@
       </c>
       <c r="R20" s="16">
         <f t="shared" si="5"/>
-        <v>0.171875</v>
+        <v>0.15625</v>
       </c>
       <c r="S20" s="19">
         <f t="shared" si="6"/>
-        <v>0.2366211810750114</v>
+        <v>0.23935677693908453</v>
       </c>
       <c r="V20" s="3" t="s">
         <v>5</v>
@@ -4505,8 +4505,8 @@
       <c r="T30" s="6">
         <v>0</v>
       </c>
-      <c r="U30" s="4">
-        <v>0.25</v>
+      <c r="U30" s="12">
+        <v>0</v>
       </c>
       <c r="W30" s="6">
         <v>1</v>
@@ -4714,7 +4714,7 @@
       </c>
       <c r="C34" s="4">
         <f t="shared" si="9"/>
-        <v>0.171875</v>
+        <v>0.15625</v>
       </c>
       <c r="E34" s="4">
         <v>0</v>
@@ -5355,7 +5355,7 @@
         <v>0.46700000000000003</v>
       </c>
       <c r="R48" s="30">
-        <v>0.60980000000000001</v>
+        <v>0.80989999999999995</v>
       </c>
       <c r="S48" s="30">
         <v>7.0489999999999997E-2</v>
@@ -5384,7 +5384,7 @@
         <v>5.2719999999999997E-6</v>
       </c>
       <c r="H49" s="31">
-        <v>4.778E-5</v>
+        <v>1.33E-5</v>
       </c>
       <c r="I49" s="31">
         <v>4.3399999999999998E-5</v>

</xml_diff>

<commit_message>
Changed table layout for easier analysis
</commit_message>
<xml_diff>
--- a/Documents/Experimentos/02/Results.xlsx
+++ b/Documents/Experimentos/02/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Volunteers" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="64">
   <si>
     <t>Q3</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>Normality: Shapiro-Wilk</t>
+  </si>
+  <si>
+    <t>Normality: Shapiro-Wilk no Outliers</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -2762,10 +2765,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:AA51"/>
+  <dimension ref="A2:AA59"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V58" sqref="V58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5364,7 +5367,7 @@
         <v>3.5950000000000003E-2</v>
       </c>
     </row>
-    <row r="49" spans="2:20">
+    <row r="49" spans="2:24">
       <c r="B49" s="28" t="s">
         <v>47</v>
       </c>
@@ -5420,9 +5423,107 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="2:20">
+    <row r="51" spans="2:24">
       <c r="B51" s="35" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="2:24">
+      <c r="P56" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q56" s="33"/>
+      <c r="R56" s="33"/>
+      <c r="S56" s="33"/>
+      <c r="T56" s="34"/>
+      <c r="U56" s="34"/>
+      <c r="V56" s="34"/>
+      <c r="W56" s="34"/>
+      <c r="X56" s="34"/>
+    </row>
+    <row r="57" spans="2:24">
+      <c r="P57" s="28"/>
+      <c r="Q57" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="R57" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="S57" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="T57" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="U57" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="V57" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="W57" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="X57" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="2:24">
+      <c r="P58" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q58" s="29">
+        <v>4.3399999999999998E-5</v>
+      </c>
+      <c r="R58" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="S58" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="T58" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="U58" s="29">
+        <v>2.5660000000000002E-5</v>
+      </c>
+      <c r="V58" s="29">
+        <v>3.4809999999999998E-6</v>
+      </c>
+      <c r="W58" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="X58" s="30">
+        <v>4.3369999999999999E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:24">
+      <c r="P59" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q59" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="R59" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="S59" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="T59" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="U59" s="31">
+        <v>5.2719999999999997E-6</v>
+      </c>
+      <c r="V59" s="31">
+        <v>1.33E-5</v>
+      </c>
+      <c r="W59" s="31">
+        <v>4.3399999999999998E-5</v>
+      </c>
+      <c r="X59" s="32">
+        <v>0.73629999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed a tab in Results.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Experimentos/02/Results.xlsx
+++ b/Documents/Experimentos/02/Results.xlsx
@@ -4,22 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Volunteers" sheetId="4" r:id="rId1"/>
-    <sheet name="Replay" sheetId="1" r:id="rId2"/>
-    <sheet name="Prov" sheetId="2" r:id="rId3"/>
-    <sheet name="Summary" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="8" r:id="rId6"/>
+    <sheet name="Volunteers characterization" sheetId="7" r:id="rId2"/>
+    <sheet name="Replay" sheetId="1" r:id="rId3"/>
+    <sheet name="Prov" sheetId="2" r:id="rId4"/>
+    <sheet name="Summary" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="75">
   <si>
     <t>Q3</t>
   </si>
@@ -244,15 +243,6 @@
   </si>
   <si>
     <t>Does discipline</t>
-  </si>
-  <si>
-    <t>Correct</t>
-  </si>
-  <si>
-    <t>Half</t>
-  </si>
-  <si>
-    <t>Wrong</t>
   </si>
 </sst>
 </file>
@@ -308,7 +298,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,18 +401,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -464,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -565,16 +543,6 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,9 +585,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.19395536825502446"/>
-          <c:y val="0.46140419947506561"/>
-          <c:w val="0.63399849666678987"/>
-          <c:h val="0.37645487022455526"/>
+          <c:y val="0.46140419947506567"/>
+          <c:w val="0.6339984966667902"/>
+          <c:h val="0.37645487022455543"/>
         </c:manualLayout>
       </c:layout>
       <c:pie3DChart>
@@ -633,7 +601,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$1:$F$1</c:f>
+              <c:f>'Volunteers characterization'!$B$1:$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -656,7 +624,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$F$2</c:f>
+              <c:f>'Volunteers characterization'!$B$2:$F$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -692,7 +660,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -736,9 +704,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.2406611496097727"/>
-          <c:y val="0.37385995411929351"/>
+          <c:y val="0.37385995411929357"/>
           <c:w val="0.5202310085846269"/>
-          <c:h val="0.60603944078468908"/>
+          <c:h val="0.60603944078468919"/>
         </c:manualLayout>
       </c:layout>
       <c:pie3DChart>
@@ -748,7 +716,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$P$1:$U$1</c:f>
+              <c:f>'Volunteers characterization'!$P$1:$U$1</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -774,7 +742,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$P$2:$U$2</c:f>
+              <c:f>'Volunteers characterization'!$P$2:$U$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -800,7 +768,6 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
       </c:pie3DChart>
     </c:plotArea>
     <c:legend>
@@ -811,7 +778,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -834,7 +801,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$P$1:$U$1</c:f>
+              <c:f>'Volunteers characterization'!$P$1:$U$1</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -860,7 +827,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$P$2:$U$2</c:f>
+              <c:f>'Volunteers characterization'!$P$2:$U$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -887,25 +854,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="100641408"/>
-        <c:axId val="95273344"/>
+        <c:axId val="93629824"/>
+        <c:axId val="98505856"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="100641408"/>
+        <c:axId val="93629824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95273344"/>
+        <c:crossAx val="98505856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95273344"/>
+        <c:axId val="98505856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +880,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100641408"/>
+        <c:crossAx val="93629824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -926,587 +893,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Number of correct , half correct, and wrong answers</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
-    <c:view3D>
-      <c:rAngAx val="1"/>
-    </c:view3D>
-    <c:plotArea>
-      <c:layout/>
-      <c:bar3DChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet3!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Prov</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Sheet3!$B$1:$AB$2</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="27"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Wrong</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Half</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Correct</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Wrong</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Half</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Correct</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Wrong</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Half</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Correct</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Wrong</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Half</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>Correct</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>Wrong</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>Half</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>Correct</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Wrong</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>Half</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>Correct</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>Wrong</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>Half</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>Correct</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Q3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Q4</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Q5</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Q6</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>Q7</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Q8</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>Q9</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet3!$B$3:$AB$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>13</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet3!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Replay</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Sheet3!$B$1:$AB$2</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="27"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Wrong</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Half</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Correct</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Wrong</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Half</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Correct</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Wrong</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Half</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Correct</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Wrong</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Half</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>Correct</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>Wrong</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>Half</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>Correct</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Wrong</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>Half</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>Correct</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>Wrong</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>Half</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>Correct</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Q3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Q4</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Q5</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Q6</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>Q7</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Q8</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>Q9</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet3!$B$4:$AB$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:shape val="box"/>
-        <c:axId val="92465408"/>
-        <c:axId val="94286208"/>
-        <c:axId val="0"/>
-      </c:bar3DChart>
-      <c:catAx>
-        <c:axId val="92465408"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94286208"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="94286208"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92465408"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>22412</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>41462</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>108137</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9155206" y="9547412"/>
-          <a:ext cx="1229285" cy="466725"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>13608</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>403437</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>149678</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1032" name="Picture 8"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="666751" y="9919607"/>
-          <a:ext cx="8350007" cy="4517571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1601,36 +994,97 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>41462</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>108137</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9155206" y="9547412"/>
+          <a:ext cx="1229285" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>13608</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>403437</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>149678</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1032" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="666751" y="9919607"/>
+          <a:ext cx="8350007" cy="4517571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2243,6 +1697,462 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:U42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="6.7109375" style="38" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" style="38" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="38" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21">
+      <c r="B1" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="2:21">
+      <c r="B2" s="41">
+        <f>SUM(B4:B42)</f>
+        <v>31</v>
+      </c>
+      <c r="C2" s="41">
+        <f>SUM(C4:C42)</f>
+        <v>6</v>
+      </c>
+      <c r="D2" s="41">
+        <f>SUM(D4:D42)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="41">
+        <f>SUM(E4:E42)</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="41">
+        <f>SUM(F4:F42)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2">
+        <v>0</v>
+      </c>
+      <c r="U2" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="2:21">
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="2:21">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="2:21">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:21">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:21">
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:21">
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:21">
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:21">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:21">
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="2:21">
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:21">
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="2:21">
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="2:21">
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="4">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="4">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="4">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4">
+        <v>1</v>
+      </c>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="4">
+        <v>1</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="4">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" s="4">
+        <v>1</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" s="4">
+        <v>1</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="4">
+        <v>1</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2955,7 +2865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O22"/>
   <sheetViews>
@@ -3801,12 +3711,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AA59"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:Q21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V45" sqref="V45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6577,765 +6487,4 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:U42"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="6.7109375" style="38" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" style="38" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" style="38" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:21">
-      <c r="B1" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="2:21">
-      <c r="B2" s="41">
-        <f>SUM(B4:B42)</f>
-        <v>31</v>
-      </c>
-      <c r="C2" s="41">
-        <f>SUM(C4:C42)</f>
-        <v>6</v>
-      </c>
-      <c r="D2" s="41">
-        <f>SUM(D4:D42)</f>
-        <v>1</v>
-      </c>
-      <c r="E2" s="41">
-        <f>SUM(E4:E42)</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="41">
-        <f>SUM(F4:F42)</f>
-        <v>0</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2">
-        <v>0</v>
-      </c>
-      <c r="U2" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="2:21">
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="2:21">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="2:21">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="2:21">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="2:21">
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="2:21">
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="2:21">
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="2:21">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="2:21">
-      <c r="B12" s="4">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="2:21">
-      <c r="B13" s="4">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="2:21">
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="2:21">
-      <c r="B15" s="4">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="2:21">
-      <c r="B16" s="4">
-        <v>1</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="4">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="4">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4">
-        <v>1</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="4">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="9"/>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="9"/>
-    </row>
-    <row r="24" spans="2:6">
-      <c r="B24" s="4">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="B25" s="4">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="B26" s="4">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="2:6">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4">
-        <v>1</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="9"/>
-    </row>
-    <row r="29" spans="2:6">
-      <c r="B29" s="4">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="9"/>
-    </row>
-    <row r="30" spans="2:6">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4">
-        <v>1</v>
-      </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="2:6">
-      <c r="B31" s="4">
-        <v>1</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="9"/>
-    </row>
-    <row r="32" spans="2:6">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4">
-        <v>1</v>
-      </c>
-      <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="B33" s="4">
-        <v>1</v>
-      </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="2:6">
-      <c r="B34" s="4">
-        <v>1</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" spans="2:6">
-      <c r="B35" s="4">
-        <v>1</v>
-      </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="9"/>
-    </row>
-    <row r="36" spans="2:6">
-      <c r="B36" s="4">
-        <v>1</v>
-      </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="9"/>
-    </row>
-    <row r="37" spans="2:6">
-      <c r="B37" s="4">
-        <v>1</v>
-      </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="9"/>
-    </row>
-    <row r="38" spans="2:6">
-      <c r="B38" s="4">
-        <v>1</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="2:6">
-      <c r="B39" s="4">
-        <v>1</v>
-      </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="9"/>
-    </row>
-    <row r="40" spans="2:6">
-      <c r="B40" s="4">
-        <v>1</v>
-      </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="9"/>
-    </row>
-    <row r="41" spans="2:6">
-      <c r="B41" s="4">
-        <v>1</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="9"/>
-    </row>
-    <row r="42" spans="2:6">
-      <c r="B42" s="4">
-        <v>1</v>
-      </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="16" max="16" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:28">
-      <c r="B1" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="F1" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="J1" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="N1" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="R1" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="V1" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Z1" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="42"/>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="B2" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="S2" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="T2" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="V2" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="W2" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="X2" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z2" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA2" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB2" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28">
-      <c r="A3" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="44">
-        <v>8</v>
-      </c>
-      <c r="C3" s="44">
-        <v>0</v>
-      </c>
-      <c r="D3" s="44">
-        <v>8</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="44">
-        <v>1</v>
-      </c>
-      <c r="G3" s="44">
-        <v>0</v>
-      </c>
-      <c r="H3" s="44">
-        <v>15</v>
-      </c>
-      <c r="I3" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="44">
-        <v>13</v>
-      </c>
-      <c r="K3" s="44">
-        <v>0</v>
-      </c>
-      <c r="L3" s="44">
-        <v>3</v>
-      </c>
-      <c r="M3" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" s="44">
-        <v>0</v>
-      </c>
-      <c r="O3" s="44">
-        <v>0</v>
-      </c>
-      <c r="P3" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="R3" s="44">
-        <v>10</v>
-      </c>
-      <c r="S3" s="44">
-        <v>0</v>
-      </c>
-      <c r="T3" s="44">
-        <v>6</v>
-      </c>
-      <c r="U3" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="V3" s="44">
-        <v>0</v>
-      </c>
-      <c r="W3" s="44">
-        <v>3</v>
-      </c>
-      <c r="X3" s="44">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z3" s="44">
-        <v>5</v>
-      </c>
-      <c r="AA3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="44">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28">
-      <c r="A4" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="44">
-        <v>15</v>
-      </c>
-      <c r="C4" s="44">
-        <v>0</v>
-      </c>
-      <c r="D4" s="44">
-        <v>1</v>
-      </c>
-      <c r="E4" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="44">
-        <v>2</v>
-      </c>
-      <c r="G4" s="44">
-        <v>0</v>
-      </c>
-      <c r="H4" s="44">
-        <v>14</v>
-      </c>
-      <c r="I4" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" s="44">
-        <v>13</v>
-      </c>
-      <c r="K4" s="44">
-        <v>0</v>
-      </c>
-      <c r="L4" s="44">
-        <v>3</v>
-      </c>
-      <c r="M4" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="44">
-        <v>0</v>
-      </c>
-      <c r="O4" s="44">
-        <v>0</v>
-      </c>
-      <c r="P4" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="R4" s="44">
-        <v>12</v>
-      </c>
-      <c r="S4" s="44">
-        <v>0</v>
-      </c>
-      <c r="T4" s="44">
-        <v>4</v>
-      </c>
-      <c r="U4" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="V4" s="44">
-        <v>0</v>
-      </c>
-      <c r="W4" s="44">
-        <v>3</v>
-      </c>
-      <c r="X4" s="44">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z4" s="44">
-        <v>8</v>
-      </c>
-      <c r="AA4" s="44">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="44">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>